<commit_message>
Data Formattion and Exploration Finished
</commit_message>
<xml_diff>
--- a/data/indexes.xlsx
+++ b/data/indexes.xlsx
@@ -5,15 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\mutla\Documents\DEERS\4 fall\430\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\gitHub\emu430-fall2023-team-4k1e_rda\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209DAEDE-763F-49F6-867E-4178924FCDA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1FCF019-FDB1-45DE-BDE8-8D2D7911A274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="2115" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3072" yWindow="1212" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="2017-2013" sheetId="1" r:id="rId1"/>
+    <sheet name="2012-2011" sheetId="2" r:id="rId2"/>
+    <sheet name="2020-2018" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="29">
   <si>
     <t>Other crimes</t>
   </si>
@@ -103,6 +105,15 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Opposition to cheque laws</t>
+  </si>
+  <si>
+    <t>Crimes related with firearms and knifes</t>
   </si>
 </sst>
 </file>
@@ -448,147 +459,433 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1C4FDE9-E97D-44CA-A623-9D50A597844D}">
+  <dimension ref="A1:A23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="45.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE0C8303-4A76-4555-8568-2327B7AC853A}">
+  <dimension ref="A1:A27"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="40" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>